<commit_message>
removed app.py in case that was causing problems
</commit_message>
<xml_diff>
--- a/phonetics/data/words.xlsx
+++ b/phonetics/data/words.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becks\Documents\Beck\Programming\Phonetics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becks\Documents\Beck\Programming\Phonetics\phonetics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{171928FA-3D72-4026-9D94-14EFAE44D55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C410AFC9-FCFD-46BC-9839-4B348794C749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="555" windowWidth="14400" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="28800" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="120">
   <si>
     <t>text</t>
   </si>
@@ -315,6 +315,87 @@
   </si>
   <si>
     <t>duck</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>mop</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>nose</t>
+  </si>
+  <si>
+    <t>piano</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>watch</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>cap</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yoghurt</t>
+  </si>
+  <si>
+    <t>frog</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>giraffe</t>
+  </si>
+  <si>
+    <t>doll</t>
+  </si>
+  <si>
+    <t>ladder</t>
+  </si>
+  <si>
+    <t>slide</t>
+  </si>
+  <si>
+    <t>pyjamas</t>
+  </si>
+  <si>
+    <t>fridge</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>sock</t>
+  </si>
+  <si>
+    <t>dress</t>
+  </si>
+  <si>
+    <t>grass</t>
+  </si>
+  <si>
+    <t>balloon</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>ll</t>
   </si>
 </sst>
 </file>
@@ -370,10 +451,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}" name="Table1" displayName="Table1" ref="A1:G55" totalsRowShown="0">
-  <autoFilter ref="A1:G55" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G55">
-    <sortCondition ref="A1:A55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}" name="Table1" displayName="Table1" ref="A1:G81" totalsRowShown="0">
+  <autoFilter ref="A1:G81" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G103">
+    <sortCondition ref="A1:A103"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A47D852A-7CBE-47BE-8813-7727A706C54B}" name="text"/>
@@ -705,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BADAE3-B698-4EA3-B37F-766E4CE3D0E8}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,649 +825,487 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
+      <c r="C6" t="s">
+        <v>119</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
+      <c r="F6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>86</v>
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" t="s">
-        <v>2</v>
-      </c>
-      <c r="G30" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
         <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>5</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G41" t="s">
         <v>2</v>
@@ -1394,191 +1313,513 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>4</v>
-      </c>
-      <c r="G49" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
-      </c>
-      <c r="B54" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" t="s">
+        <v>89</v>
+      </c>
+      <c r="E66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>55</v>
+      </c>
+      <c r="B69" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>27</v>
+      </c>
+      <c r="F69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>46</v>
+      </c>
+      <c r="B77" t="s">
+        <v>85</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="s">
+        <v>85</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+      <c r="E80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>50</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B81" t="s">
         <v>32</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D81" t="s">
         <v>5</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E81" t="s">
         <v>32</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G81" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
colours sort of working but not based on placement in word
</commit_message>
<xml_diff>
--- a/phonetics/data/words.xlsx
+++ b/phonetics/data/words.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becks\Documents\Beck\Programming\Phonetics\phonetics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C410AFC9-FCFD-46BC-9839-4B348794C749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4D1FB7-D8FD-4397-9876-F08B2B806CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="555" windowWidth="28800" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="17565" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="132">
   <si>
     <t>text</t>
   </si>
@@ -311,9 +311,6 @@
     <t xml:space="preserve">s </t>
   </si>
   <si>
-    <t>th(is)</t>
-  </si>
-  <si>
     <t>duck</t>
   </si>
   <si>
@@ -396,6 +393,45 @@
   </si>
   <si>
     <t>ll</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c </t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>dge</t>
+  </si>
+  <si>
+    <t>ffe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t </t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ge</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b </t>
   </si>
 </sst>
 </file>
@@ -451,10 +487,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}" name="Table1" displayName="Table1" ref="A1:G81" totalsRowShown="0">
-  <autoFilter ref="A1:G81" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G103">
-    <sortCondition ref="A1:A103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}" name="Table1" displayName="Table1" ref="A1:G80" totalsRowShown="0">
+  <autoFilter ref="A1:G80" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G102">
+    <sortCondition ref="A1:A102"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A47D852A-7CBE-47BE-8813-7727A706C54B}" name="text"/>
@@ -786,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BADAE3-B698-4EA3-B37F-766E4CE3D0E8}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,10 +861,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -836,13 +872,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -899,7 +935,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -961,12 +997,30 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,7 +1028,7 @@
         <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
@@ -1019,7 +1073,7 @@
         <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1044,17 +1098,41 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1088,224 +1166,356 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
-        <v>91</v>
+      <c r="D22" t="s">
+        <v>21</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="F22" t="s">
-        <v>25</v>
+      <c r="G22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="D23" t="s">
-        <v>21</v>
+      <c r="C23" t="s">
+        <v>4</v>
       </c>
       <c r="E23" t="s">
         <v>9</v>
       </c>
-      <c r="G23" t="s">
-        <v>28</v>
+      <c r="F23" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
+      <c r="D24" t="s">
+        <v>87</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="F24" t="s">
-        <v>4</v>
+      <c r="G24" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34" t="s">
-        <v>118</v>
+      <c r="D34" t="s">
+        <v>27</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
       </c>
-      <c r="F34" t="s">
-        <v>5</v>
+      <c r="G34" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
         <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>3</v>
+        <v>31</v>
+      </c>
+      <c r="F37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
       </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
       <c r="E38" t="s">
         <v>31</v>
       </c>
+      <c r="G38" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
-      </c>
-      <c r="G39" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G41" t="s">
         <v>2</v>
@@ -1313,386 +1523,473 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>33</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="D46" t="s">
-        <v>89</v>
+      <c r="C46" t="s">
+        <v>125</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
       </c>
-      <c r="G46" t="s">
-        <v>26</v>
+      <c r="F46" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>2</v>
       </c>
-      <c r="D48" t="s">
-        <v>27</v>
-      </c>
       <c r="E48" t="s">
         <v>2</v>
-      </c>
-      <c r="G48" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="G50" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
       </c>
-      <c r="D52" t="s">
-        <v>2</v>
-      </c>
       <c r="E52" t="s">
         <v>5</v>
       </c>
-      <c r="G52" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
       <c r="E53" t="s">
         <v>5</v>
       </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>48</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
       </c>
-      <c r="D55" t="s">
-        <v>7</v>
+      <c r="C55" t="s">
+        <v>19</v>
       </c>
       <c r="E55" t="s">
         <v>5</v>
       </c>
-      <c r="G55" t="s">
-        <v>7</v>
+      <c r="F55" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
         <v>22</v>
       </c>
-      <c r="C57" t="s">
-        <v>6</v>
+      <c r="D57" t="s">
+        <v>18</v>
       </c>
       <c r="E57" t="s">
         <v>22</v>
       </c>
-      <c r="F57" t="s">
-        <v>6</v>
+      <c r="G57" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D58" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G58" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
         <v>21</v>
       </c>
       <c r="D59" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E59" t="s">
         <v>28</v>
       </c>
       <c r="G59" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>90</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>28</v>
+        <v>90</v>
+      </c>
+      <c r="F60" t="s">
+        <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>129</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E61" t="s">
-        <v>90</v>
-      </c>
-      <c r="F61" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G61" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
       </c>
       <c r="G63" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>20</v>
+      </c>
+      <c r="G64" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
-        <v>20</v>
-      </c>
-      <c r="G65" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
         <v>89</v>
       </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
       <c r="E66" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="G66" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="E67" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
         <v>27</v>
       </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
       <c r="E68" t="s">
         <v>27</v>
       </c>
+      <c r="F68" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
-      </c>
-      <c r="C69" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>27</v>
-      </c>
-      <c r="F69" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="G69" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
         <v>24</v>
       </c>
-      <c r="D70" t="s">
-        <v>2</v>
-      </c>
       <c r="E70" t="s">
         <v>24</v>
       </c>
-      <c r="G70" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
         <v>24</v>
@@ -1703,123 +2000,148 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>88</v>
       </c>
       <c r="E72" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="G72" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>99</v>
+        <v>43</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B74" t="s">
         <v>4</v>
       </c>
-      <c r="D74" t="s">
-        <v>6</v>
-      </c>
       <c r="E74" t="s">
         <v>4</v>
       </c>
-      <c r="G74" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
       </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
       <c r="E75" t="s">
         <v>4</v>
       </c>
+      <c r="G75" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B76" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" t="s">
+        <v>118</v>
+      </c>
+      <c r="D76" t="s">
         <v>4</v>
       </c>
-      <c r="D76" t="s">
-        <v>10</v>
-      </c>
       <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
+        <v>23</v>
+      </c>
+      <c r="G76" t="s">
         <v>4</v>
-      </c>
-      <c r="G76" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
         <v>85</v>
       </c>
-      <c r="D77" t="s">
-        <v>4</v>
-      </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
-      <c r="G77" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="B78" t="s">
         <v>85</v>
       </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
+      <c r="F78" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>81</v>
+      </c>
+      <c r="B79" t="s">
+        <v>32</v>
+      </c>
+      <c r="C79" t="s">
+        <v>131</v>
+      </c>
+      <c r="E79" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
         <v>32</v>
       </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
       <c r="E80" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" t="s">
-        <v>32</v>
-      </c>
-      <c r="D81" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" t="s">
-        <v>32</v>
-      </c>
-      <c r="G81" t="s">
+      <c r="G80" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed error with red and also removed spaces in data causing errors
</commit_message>
<xml_diff>
--- a/phonetics/data/words.xlsx
+++ b/phonetics/data/words.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becks\Documents\Beck\Programming\Phonetics\phonetics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4D1FB7-D8FD-4397-9876-F08B2B806CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DC2CA-64C7-4A76-ADCF-BA842CCC575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="555" windowWidth="17565" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
+    <workbookView xWindow="14400" yWindow="555" windowWidth="14400" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="126">
   <si>
     <t>text</t>
   </si>
@@ -296,9 +296,6 @@
     <t>y</t>
   </si>
   <si>
-    <t xml:space="preserve">m </t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>th</t>
   </si>
   <si>
-    <t xml:space="preserve">s </t>
-  </si>
-  <si>
     <t>duck</t>
   </si>
   <si>
@@ -398,9 +392,6 @@
     <t>ss</t>
   </si>
   <si>
-    <t xml:space="preserve">c </t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -410,9 +401,6 @@
     <t>ffe</t>
   </si>
   <si>
-    <t xml:space="preserve">t </t>
-  </si>
-  <si>
     <t>mm</t>
   </si>
   <si>
@@ -425,13 +413,7 @@
     <t>bb</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>ck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b </t>
   </si>
 </sst>
 </file>
@@ -824,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BADAE3-B698-4EA3-B37F-766E4CE3D0E8}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,10 +843,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -872,13 +854,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -901,7 +883,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -997,10 +979,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1014,10 +996,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1028,7 +1010,7 @@
         <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
@@ -1045,7 +1027,7 @@
         <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -1056,7 +1038,7 @@
         <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -1073,7 +1055,7 @@
         <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1098,13 +1080,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1115,13 +1097,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
@@ -1132,7 +1114,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1172,7 +1154,7 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
@@ -1223,24 +1205,24 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
@@ -1251,7 +1233,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -1268,13 +1250,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E27" t="s">
         <v>31</v>
@@ -1302,13 +1284,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -1319,7 +1301,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -1336,13 +1318,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
@@ -1353,19 +1335,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1376,7 +1358,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
@@ -1387,7 +1369,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1444,7 +1426,7 @@
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E37" t="s">
         <v>31</v>
@@ -1472,13 +1454,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
         <v>23</v>
@@ -1523,7 +1505,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -1557,7 +1539,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -1580,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
         <v>1</v>
@@ -1597,13 +1579,13 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1625,7 +1607,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
         <v>2</v>
@@ -1653,10 +1635,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G50" t="s">
         <v>31</v>
@@ -1692,7 +1674,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -1726,7 +1708,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -1749,7 +1731,7 @@
         <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
         <v>22</v>
@@ -1800,7 +1782,7 @@
         <v>21</v>
       </c>
       <c r="D59" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="E59" t="s">
         <v>28</v>
@@ -1814,7 +1796,7 @@
         <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -1823,7 +1805,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="F60" t="s">
         <v>2</v>
@@ -1834,13 +1816,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B61" t="s">
         <v>20</v>
-      </c>
-      <c r="C61" t="s">
-        <v>129</v>
       </c>
       <c r="D61" t="s">
         <v>18</v>
@@ -1871,13 +1850,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
@@ -1908,7 +1887,7 @@
         <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E65" t="s">
         <v>25</v>
@@ -1919,7 +1898,7 @@
         <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
@@ -2000,13 +1979,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E72" t="s">
         <v>4</v>
@@ -2068,7 +2047,7 @@
         <v>85</v>
       </c>
       <c r="C76" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D76" t="s">
         <v>4</v>
@@ -2096,7 +2075,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
         <v>85</v>
@@ -2119,7 +2098,7 @@
         <v>32</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="E79" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Got form set up, goes from home page then testing. Not done results. Not tested entry without form
</commit_message>
<xml_diff>
--- a/phonetics/data/words.xlsx
+++ b/phonetics/data/words.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becks\Documents\Beck\Programming\Phonetics\phonetics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DC2CA-64C7-4A76-ADCF-BA842CCC575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF33D63-C070-4A3C-A398-C26B2CEAB316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="555" windowWidth="14400" windowHeight="17445" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
+    <workbookView xWindow="14400" yWindow="9330" windowWidth="14400" windowHeight="8670" xr2:uid="{FFA59960-26CE-45B2-83F4-1B76359CC4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="130">
   <si>
     <t>text</t>
   </si>
@@ -414,6 +414,18 @@
   </si>
   <si>
     <t>ck</t>
+  </si>
+  <si>
+    <t>image_credit</t>
+  </si>
+  <si>
+    <t>Image by &lt;a href="https://pixabay.com/users/clker-free-vector-images-3736/?utm_source=link-attribution&amp;utm_medium=referral&amp;utm_campaign=image&amp;utm_content=303699"&gt;Clker-Free-Vector-Images&lt;/a&gt; from &lt;a href="https://pixabay.com//?utm_source=link-attribution&amp;utm_medium=referral&amp;utm_campaign=image&amp;utm_content=303699"&gt;Pixabay&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>image_link</t>
+  </si>
+  <si>
+    <t>https://cdn.pixabay.com/photo/2014/04/02/10/23/lion-303699_960_720.png</t>
   </si>
 </sst>
 </file>
@@ -469,12 +481,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}" name="Table1" displayName="Table1" ref="A1:G80" totalsRowShown="0">
-  <autoFilter ref="A1:G80" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}" name="Table1" displayName="Table1" ref="A1:I80" totalsRowShown="0">
+  <autoFilter ref="A1:I80" xr:uid="{A8C0B577-888C-438C-822F-A4651F6DEB80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G102">
     <sortCondition ref="A1:A102"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A47D852A-7CBE-47BE-8813-7727A706C54B}" name="text"/>
     <tableColumn id="2" xr3:uid="{0EED4A6F-019A-400B-808C-4F0B56928F96}" name="initial"/>
     <tableColumn id="3" xr3:uid="{6077724E-5664-4D1E-80A1-810A61C2675A}" name="medial"/>
@@ -482,6 +494,8 @@
     <tableColumn id="5" xr3:uid="{5907FD7F-AEC5-4695-A7FF-1784303E8B47}" name="initial_phoneme"/>
     <tableColumn id="6" xr3:uid="{C4C5DACF-1613-463E-AB30-01AF1CBF5B1D}" name="medial_phoneme"/>
     <tableColumn id="7" xr3:uid="{669ADE36-19E2-4984-8EF2-904CBDD33455}" name="final_phoneme"/>
+    <tableColumn id="8" xr3:uid="{C440C847-1D76-4E69-9561-B66CF45C5D48}" name="image_credit"/>
+    <tableColumn id="9" xr3:uid="{289A515B-83B8-4607-AF52-19F6CC7E3995}" name="image_link"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -804,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BADAE3-B698-4EA3-B37F-766E4CE3D0E8}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +832,7 @@
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,8 +854,14 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -852,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -875,7 +895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -892,7 +912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -909,7 +929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -926,7 +946,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -943,7 +963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -960,7 +980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -977,7 +997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -994,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -1005,7 +1025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1022,7 +1042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1033,7 +1053,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1050,7 +1070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1061,7 +1081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1350,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1367,7 +1387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>95</v>
       </c>
@@ -1384,7 +1404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1401,7 +1421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1418,7 +1438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1435,7 +1455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -1452,7 +1472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>106</v>
       </c>
@@ -1469,7 +1489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1485,8 +1505,14 @@
       <c r="G40" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>127</v>
+      </c>
+      <c r="I40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1503,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -1520,7 +1546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1537,7 +1563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -1554,7 +1580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -1571,7 +1597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1588,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -1605,7 +1631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>

</xml_diff>